<commit_message>
fiz algumas mudanças no dados
</commit_message>
<xml_diff>
--- a/santander.xlsx
+++ b/santander.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manucirne\Documents\CD\Projeto2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manucirne\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1433,7 +1433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1453,14 +1453,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1501,7 +1493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1509,7 +1501,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1850,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164:A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1944,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2249,7 +2240,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2377,7 +2368,7 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -2433,7 +2424,7 @@
         <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -2473,7 +2464,7 @@
         <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -2529,7 +2520,7 @@
         <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -2625,7 +2616,7 @@
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -3033,7 +3024,7 @@
         <v>135</v>
       </c>
       <c r="B147" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -3049,7 +3040,7 @@
         <v>137</v>
       </c>
       <c r="B149" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -3105,7 +3096,7 @@
         <v>144</v>
       </c>
       <c r="B156" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -3144,7 +3135,7 @@
       <c r="A161" t="s">
         <v>148</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="4" t="s">
         <v>455</v>
       </c>
     </row>
@@ -4273,6 +4264,7 @@
     <hyperlink ref="A95" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4280,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4403,7 +4395,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>289</v>
       </c>
       <c r="B15" t="s">

</xml_diff>